<commit_message>
Milestone 2 Commit 2
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\igm671FinalProjectGITMurphy\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\git671finalproject\igme671-Project-Final\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAE74AA-5BB8-4BA2-A2C1-6240BD2FE98B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A3EDC6-AACD-41F5-810B-3C44CD92123F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5685" yWindow="2970" windowWidth="18615" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Event Description</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Step taken by player on hard surface, perhaps stone or brick</t>
   </si>
   <si>
-    <t>Assets Requied</t>
-  </si>
-  <si>
     <t>Sound Name</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Use of random to alternate with walk 01 and 02, possibly consolidated into one sound with FMOD</t>
   </si>
   <si>
-    <t>Elastic or spring noise, noise of triumph, viscous liquid sample</t>
-  </si>
-  <si>
     <t>Intense impact onleaves, grass, brick or stone</t>
   </si>
   <si>
@@ -166,6 +160,18 @@
   </si>
   <si>
     <t>Should be similar in sound neighborhood as the above interface sound</t>
+  </si>
+  <si>
+    <t>Assets Required</t>
+  </si>
+  <si>
+    <t>Jawharp multi instrument, bubbling mud sample</t>
+  </si>
+  <si>
+    <t>5 different possible jawharp twangs, -/+ .25 semitones</t>
+  </si>
+  <si>
+    <t>Iteration 1</t>
   </si>
 </sst>
 </file>
@@ -543,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,17 +561,17 @@
     <col min="4" max="4" width="33.140625" customWidth="1"/>
     <col min="5" max="5" width="69.7109375" customWidth="1"/>
     <col min="6" max="6" width="73.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="87.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -574,13 +580,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -594,10 +600,10 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -611,10 +617,10 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -625,10 +631,10 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -639,10 +645,10 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -653,10 +659,16 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -667,10 +679,10 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -681,10 +693,10 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -695,10 +707,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -712,15 +724,15 @@
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>9</v>
@@ -729,42 +741,42 @@
         <v>14</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="F13" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="H14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Milestone 3 further commits
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\git671finalproject\igme671-Project-Final\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD04BBD8-F81E-49F7-AB50-25222AF061E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AAFA7F-FEBD-4370-8578-44EFDA4BFC65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>Event Description</t>
   </si>
@@ -69,18 +69,12 @@
     <t>LandOnGround</t>
   </si>
   <si>
-    <t>Step taken by player on hard surface, perhaps stone or brick</t>
-  </si>
-  <si>
     <t>Sound Name</t>
   </si>
   <si>
     <t>Crystalline ring when gem is collected.</t>
   </si>
   <si>
-    <t>Sloshing noise as player reforms.</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -93,18 +87,9 @@
     <t>Walk 03</t>
   </si>
   <si>
-    <t>Crunch of leaves/grass/impact on stone</t>
-  </si>
-  <si>
     <t>Player leaps into the air.</t>
   </si>
   <si>
-    <t>Viscous liquid sample</t>
-  </si>
-  <si>
-    <t>Chime, bell or ding sound</t>
-  </si>
-  <si>
     <t>Wind, chirping of birds</t>
   </si>
   <si>
@@ -174,7 +159,34 @@
     <t>Footsteps in mud</t>
   </si>
   <si>
-    <t>Up to 6 possible squelching noises in mud, -/+ .25 semitones</t>
+    <t>See Music</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Parameterized music, gaining intensity as player loses health.</t>
+  </si>
+  <si>
+    <t>Noise of distress recording, dry puff recording,  raspberry recording</t>
+  </si>
+  <si>
+    <t>All sounds personally recorded</t>
+  </si>
+  <si>
+    <t>Up to 5/6 possible squelching noises in mud, -/+ .25 semitones</t>
+  </si>
+  <si>
+    <t>See Walk 01</t>
+  </si>
+  <si>
+    <t>Step taken by semi solid player</t>
+  </si>
+  <si>
+    <t>Airliner bell</t>
+  </si>
+  <si>
+    <t>Sloshing noise as player disappears.</t>
   </si>
 </sst>
 </file>
@@ -550,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H14"/>
+  <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,10 +583,10 @@
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -583,13 +595,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -600,13 +612,13 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H3" t="s">
         <v>49</v>
@@ -619,14 +631,11 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -637,13 +646,13 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -654,10 +663,10 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -668,16 +677,16 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -688,10 +697,10 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -702,10 +711,16 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -716,10 +731,13 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>52</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -733,58 +751,72 @@
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Milestone 4 further commit
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\git671finalproject\igme671-Project-Final\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B617DDAB-A3E2-49E6-9EAC-8E33FDBBF163}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37B4D1C-3AD9-49D2-A0D2-284CDDE4E54F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>Event Description</t>
   </si>
@@ -99,12 +99,6 @@
     <t>Player stomps on the enemy.</t>
   </si>
   <si>
-    <t>Viscous liquid sample, noise of surprise</t>
-  </si>
-  <si>
-    <t>Intense impact onleaves, grass, brick or stone</t>
-  </si>
-  <si>
     <t>Sounds that will be replacing default sounds upon completion status.</t>
   </si>
   <si>
@@ -123,12 +117,6 @@
     <t>Mousing over a pause menu button.</t>
   </si>
   <si>
-    <t>Possible Rubbery noise</t>
-  </si>
-  <si>
-    <t>Possible rubbery noise</t>
-  </si>
-  <si>
     <t>Should be similar in sound neighborhood as the above interface sound</t>
   </si>
   <si>
@@ -187,6 +175,21 @@
   </si>
   <si>
     <t>Iteration 2</t>
+  </si>
+  <si>
+    <t>Viscous liquid sample, sizzling noise</t>
+  </si>
+  <si>
+    <t>Splash in mud</t>
+  </si>
+  <si>
+    <t>Same multi instrument as Walk, needs something to differentiate from normal walking</t>
+  </si>
+  <si>
+    <t>Mustard bottle</t>
+  </si>
+  <si>
+    <t>Brief pop</t>
   </si>
 </sst>
 </file>
@@ -575,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +597,7 @@
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>
@@ -606,7 +609,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>16</v>
@@ -623,16 +626,16 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -644,10 +647,10 @@
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -661,10 +664,10 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -678,7 +681,10 @@
         <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -692,13 +698,13 @@
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -712,7 +718,13 @@
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -723,16 +735,16 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -746,10 +758,10 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -763,7 +775,7 @@
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -777,55 +789,61 @@
         <v>9</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="F13" s="5" t="s">
-        <v>32</v>
+        <v>53</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
         <v>30</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>